<commit_message>
test: Pruebas con archivo excel
</commit_message>
<xml_diff>
--- a/HU061 Matriz de Pruebas.xlsx
+++ b/HU061 Matriz de Pruebas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragdn\OneDrive\Documentos\Cacao\Requerimientos\HU061 - Cuenta Eje SAAS ES\Liberación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragdn\OneDrive\Documentos\Cacao\Requerimientos\HU061 - Cuenta Eje SAAS ES\Desarrollo\HU061_Desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A38712C-38EC-40E0-9F18-180CCD07B5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ECFC51-7B70-4C89-BDF4-6FEA5D14435F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
   <si>
     <t>Totem</t>
   </si>
@@ -599,6 +599,9 @@
 3.- Asignar el número de tarjeta, así como el monto deseado.
 4.- Ejecutar la transacción, mediante el botón "Enviar Operación".</t>
   </si>
+  <si>
+    <t>DNU</t>
+  </si>
 </sst>
 </file>
 
@@ -786,7 +789,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -856,6 +859,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1098,7 +1107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1293,6 +1302,12 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1331,11 +1346,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1900,10 +1912,10 @@
   <dimension ref="A1:J883"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="3" x14ac:dyDescent="0.2"/>
@@ -1922,17 +1934,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="22" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
       <c r="J1" s="40"/>
     </row>
     <row r="2" spans="1:10" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1940,11 +1952,11 @@
         <v>49</v>
       </c>
       <c r="B2" s="41"/>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="74"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="76"/>
       <c r="F2" s="49" t="s">
         <v>6</v>
       </c>
@@ -1960,11 +1972,11 @@
         <v>45</v>
       </c>
       <c r="B3" s="41"/>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="77"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="79"/>
       <c r="F3" s="43"/>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
@@ -1976,11 +1988,11 @@
         <v>43</v>
       </c>
       <c r="B4" s="42"/>
-      <c r="C4" s="78">
+      <c r="C4" s="80">
         <v>1</v>
       </c>
-      <c r="D4" s="79"/>
-      <c r="E4" s="80"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="82"/>
       <c r="F4" s="44"/>
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
@@ -2056,7 +2068,9 @@
       <c r="H7" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="54"/>
+      <c r="I7" s="86" t="s">
+        <v>77</v>
+      </c>
       <c r="J7" s="54"/>
     </row>
     <row r="8" spans="1:10" s="46" customFormat="1" ht="384.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2208,8 +2222,8 @@
       <c r="H14" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="84"/>
-      <c r="J14" s="85"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="71"/>
     </row>
     <row r="15" spans="1:10" ht="384.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A15" s="69">
@@ -2232,8 +2246,8 @@
       <c r="H15" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="84"/>
-      <c r="J15" s="85"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="71"/>
     </row>
     <row r="16" spans="1:10" ht="384.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A16" s="69">
@@ -2256,8 +2270,8 @@
       <c r="H16" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="84"/>
-      <c r="J16" s="85"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="71"/>
     </row>
     <row r="17" spans="1:10" ht="384.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A17" s="69">
@@ -2280,8 +2294,8 @@
       <c r="H17" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="84"/>
-      <c r="J17" s="85"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="71"/>
     </row>
     <row r="18" spans="1:10" ht="384.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A18" s="69">
@@ -2304,8 +2318,8 @@
       <c r="H18" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I18" s="84"/>
-      <c r="J18" s="85"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="71"/>
     </row>
     <row r="19" spans="1:10" ht="384.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A19" s="69">
@@ -2328,8 +2342,8 @@
       <c r="H19" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="I19" s="84"/>
-      <c r="J19" s="85"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="71"/>
     </row>
     <row r="20" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="63">
@@ -12818,14 +12832,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="83"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>

</xml_diff>

<commit_message>
test: Cambio en color de celdas
</commit_message>
<xml_diff>
--- a/HU061 Matriz de Pruebas.xlsx
+++ b/HU061 Matriz de Pruebas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo\DNU\Documentacion\HU061 Cuenta Eje SAAS en Prepago SAAS ES\Repo\HU061_Desarrollo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragdn\OneDrive\Documentos\Cacao\Requerimientos\HU061 - Cuenta Eje SAAS ES\Desarrollo\HU061_Desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C510E43-89D2-445C-8145-305A874D4828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFD9A26-A643-4E28-85D7-C9AE7EF937E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ciclo 1" sheetId="3" r:id="rId1"/>
@@ -872,7 +872,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -942,6 +942,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1184,7 +1190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1423,6 +1429,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1986,10 +1995,10 @@
   <dimension ref="A1:J883"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="3" x14ac:dyDescent="0.2"/>
@@ -2142,7 +2151,7 @@
       <c r="H7" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="54" t="s">
+      <c r="I7" s="86" t="s">
         <v>78</v>
       </c>
       <c r="J7" s="54"/>

</xml_diff>

<commit_message>
feat: Se agregan cambios a los scripts y matriz de pruebas
</commit_message>
<xml_diff>
--- a/HU061 Matriz de Pruebas.xlsx
+++ b/HU061 Matriz de Pruebas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo\DNU\Documentacion\HU061 Cuenta Eje SAAS en Prepago SAAS ES\Repo\HU061_Desarrollo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragdn\OneDrive\Documentos\Cacao\Requerimientos\HU061 - Cuenta Eje SAAS ES\Desarrollo\HU061_Desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCFDED4-1C53-4915-832D-6FC3B4D245BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A16BE20-A401-4724-8D97-C002E6606562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ciclo 1" sheetId="3" r:id="rId1"/>
@@ -600,6 +600,42 @@
 4.- Ejecutar la transacción, mediante el botón "Enviar Operación".</t>
   </si>
   <si>
+    <t>Prueba Exitosa</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Datos de la prueba___________________________
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Colectiva: 148552
+Tarjeta: 749996622114
+Monto: 100
+Saldo: 500</t>
+    </r>
+  </si>
+  <si>
+    <t>Rechazada</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
 </t>
@@ -643,47 +679,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Colectiva: 148552
-Tarjeta: 749996622114
-Monto: 100
-Saldo: 500</t>
+      <t>Colectiva:
+Tarjeta:
+Monto:
+Saldo Actual SaaS:
+Saldo Actual TH:</t>
     </r>
-  </si>
-  <si>
-    <t>Prueba Exitosa</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Datos de la prueba___________________________
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Colectiva: 148552
-Tarjeta: 749996622114
-Monto: 100
-Saldo: 500</t>
-    </r>
-  </si>
-  <si>
-    <t>Rechazada</t>
   </si>
 </sst>
 </file>
@@ -1475,55 +1476,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>91335</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>91337</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>3555709</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>4211921</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7953B597-A8A9-D61B-E065-D471FA1354ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15879349" y="17171097"/>
-          <a:ext cx="7639716" cy="4120584"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -2035,10 +1987,10 @@
   <dimension ref="A1:J883"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="3" x14ac:dyDescent="0.2"/>
@@ -2154,7 +2106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="46" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="46" customFormat="1" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A6" s="63">
         <v>1</v>
       </c>
@@ -2170,7 +2122,7 @@
       <c r="I6" s="57"/>
       <c r="J6" s="57"/>
     </row>
-    <row r="7" spans="1:10" s="46" customFormat="1" ht="384.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="46" customFormat="1" ht="384.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="56">
         <v>1.1000000000000001</v>
       </c>
@@ -2180,7 +2132,7 @@
         <v>58</v>
       </c>
       <c r="E7" s="54" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F7" s="55" t="s">
         <v>17</v>
@@ -2192,11 +2144,11 @@
         <v>60</v>
       </c>
       <c r="I7" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J7" s="54"/>
     </row>
-    <row r="8" spans="1:10" s="46" customFormat="1" ht="384.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="46" customFormat="1" ht="384.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="56">
         <v>1.2</v>
       </c>
@@ -2206,7 +2158,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="66" t="s">
         <v>17</v>
@@ -2218,11 +2170,11 @@
         <v>61</v>
       </c>
       <c r="I8" s="65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J8" s="67"/>
     </row>
-    <row r="9" spans="1:10" s="46" customFormat="1" ht="384.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="46" customFormat="1" ht="384.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="56"/>
       <c r="B9" s="65"/>
       <c r="C9" s="65"/>
@@ -2244,7 +2196,7 @@
       <c r="I9" s="65"/>
       <c r="J9" s="67"/>
     </row>
-    <row r="10" spans="1:10" s="46" customFormat="1" ht="384.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="46" customFormat="1" ht="384.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56"/>
       <c r="B10" s="65"/>
       <c r="C10" s="65"/>
@@ -2266,7 +2218,7 @@
       <c r="I10" s="65"/>
       <c r="J10" s="67"/>
     </row>
-    <row r="11" spans="1:10" s="46" customFormat="1" ht="384.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="46" customFormat="1" ht="384.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
@@ -2288,7 +2240,7 @@
       <c r="I11" s="65"/>
       <c r="J11" s="67"/>
     </row>
-    <row r="12" spans="1:10" s="46" customFormat="1" ht="384.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="46" customFormat="1" ht="384.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="56"/>
       <c r="B12" s="65"/>
       <c r="C12" s="65"/>
@@ -2336,7 +2288,7 @@
         <v>58</v>
       </c>
       <c r="E14" s="54" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="F14" s="55" t="s">
         <v>17</v>
@@ -2360,7 +2312,7 @@
         <v>59</v>
       </c>
       <c r="E15" s="54" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="F15" s="66" t="s">
         <v>17</v>
@@ -2470,7 +2422,7 @@
       <c r="I19" s="70"/>
       <c r="J19" s="71"/>
     </row>
-    <row r="20" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="22.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A20" s="63">
         <v>3</v>
       </c>
@@ -2486,7 +2438,7 @@
       <c r="I20" s="61"/>
       <c r="J20" s="62"/>
     </row>
-    <row r="21" spans="1:10" ht="384.75" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="384.75" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A21" s="68">
         <v>3.1</v>
       </c>
@@ -2510,7 +2462,7 @@
       <c r="I21" s="28"/>
       <c r="J21" s="30"/>
     </row>
-    <row r="22" spans="1:10" ht="384.75" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="384.75" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A22" s="68">
         <v>3.2</v>
       </c>
@@ -2534,7 +2486,7 @@
       <c r="I22" s="28"/>
       <c r="J22" s="30"/>
     </row>
-    <row r="23" spans="1:10" ht="384.75" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="384.75" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A23" s="68">
         <v>3.3</v>
       </c>
@@ -2558,7 +2510,7 @@
       <c r="I23" s="28"/>
       <c r="J23" s="30"/>
     </row>
-    <row r="24" spans="1:10" ht="384.75" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="384.75" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A24" s="68">
         <v>3.4</v>
       </c>
@@ -2582,7 +2534,7 @@
       <c r="I24" s="28"/>
       <c r="J24" s="30"/>
     </row>
-    <row r="25" spans="1:10" ht="384.75" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="384.75" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A25" s="68">
         <v>3.5</v>
       </c>
@@ -2606,7 +2558,7 @@
       <c r="I25" s="28"/>
       <c r="J25" s="30"/>
     </row>
-    <row r="26" spans="1:10" ht="384.75" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="384.75" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A26" s="68">
         <v>3.6</v>
       </c>
@@ -12813,8 +12765,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix: Se agregan pruebas sobre eventos de ATM
</commit_message>
<xml_diff>
--- a/HU061 Matriz de Pruebas.xlsx
+++ b/HU061 Matriz de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragdn\OneDrive\Documentos\Cacao\Requerimientos\HU061 - Cuenta Eje SAAS ES\Desarrollo\HU061_Desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A16BE20-A401-4724-8D97-C002E6606562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953D318C-69A9-41BC-8A76-5AB478D2068B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
   <si>
     <t>Totem</t>
   </si>
@@ -684,6 +684,401 @@
 Monto:
 Saldo Actual SaaS:
 Saldo Actual TH:</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+            "ImporteOrigenMovimiento": "4.5000",
+            "MonedaOrigenMovimiento": "484",
+            "NumeroAfiliacionComercio": "0000000",
+            "DescripcionComercio": "Member Financial Instis",
+            "PaisComercio": "484",
+            "DescripcionPais": "México",
+            "SaldoDespuesMovimiento": "495.50",
+            "ClaveMovimiento": "PB49",
+            "MCC": "6011",
+            "EstatusPostOperacion": "004",
+            "DescripcionPostOperacion": "EN TRANSITO",
+            "Autorizacion": "001887",
+            "IDMovimiento": "1393324",
+            "FechaMovimiento": "2022-06-20 13:43:44",
+            "ConceptoMovimiento": "RETIRO ATM SaaS",
+            "TipoMovimientoCargoAbono": "Cargo",
+            "ImporteMovimiento": "4.5000",
+            "MonedaMovimiento": "MXN",
+            "Referencia": "",
+            "Observaciones": ""
+}</t>
+  </si>
+  <si>
+    <t>{
+            "ImporteOrigenMovimiento": "5.0000",
+            "MonedaOrigenMovimiento": "484",
+            "NumeroAfiliacionComercio": "0000000",
+            "DescripcionComercio": "Member Financial Instis",
+            "PaisComercio": "484",
+            "DescripcionPais": "México",
+            "SaldoDespuesMovimiento": "495.00",
+            "ClaveMovimiento": "PB49",
+            "MCC": "6011",
+            "EstatusPostOperacion": "004",
+            "DescripcionPostOperacion": "EN TRANSITO",
+            "Autorizacion": "001888",
+            "IDMovimiento": "1393327",
+            "FechaMovimiento": "2022-06-20 14:01:41",
+            "ConceptoMovimiento": "RETIRO ATM SaaS",
+            "TipoMovimientoCargoAbono": "Cargo",
+            "ImporteMovimiento": "5.0000",
+            "MonedaMovimiento": "MXN",
+            "Referencia": "",
+            "Observaciones": ""
+        }</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Datos de la prueba___________________________
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Colectiva: Subempresa Debito Prueba SAAS
+Tarjeta: 9900012046474446
+Monto:$500.00
+Saldo Actual SaaS $1,047.50
+Saldo Actual TH: $495.00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Datos de la prueba</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>___________________________</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Colectiva: Subempresa Debito Prueba SAAS
+Tarjeta: 9900012046474446
+Monto:$5.00
+Saldo Actual SaaS $1,052.50
+Saldo Actual TH: $500.00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Datos de la prueba___________________________
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Colectiva: Empresa Debito Prueba SAAS
+Tarjeta: 9900012011858860
+Monto: $1,000.00
+Saldo Actual SaaS: $1,052.50
+Saldo Actual TH: $495.50</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Datos de la prueba</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>___________________________</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Colectiva: Empresa Debito Prueba SAAS
+Tarjeta: 9900012011858860
+Monto: $4.50
+Saldo Actual SaaS:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>$1,057.00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Saldo Actual TH: $500.00</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+            "ImporteOrigenMovimiento": "100.0000",
+            "MonedaOrigenMovimiento": "484",
+            "NumeroAfiliacionComercio": "0000000",
+            "DescripcionComercio": "Member Financial Instis",
+            "PaisComercio": "484",
+            "DescripcionPais": "México",
+            "SaldoDespuesMovimiento": "1712.80",
+            "ClaveMovimiento": "PB49",
+            "MCC": "6011",
+            "EstatusPostOperacion": "004",
+            "DescripcionPostOperacion": "EN TRANSITO",
+            "Autorizacion": "001889",
+            "IDMovimiento": "1393329",
+            "FechaMovimiento": "2022-06-20 14:12:00",
+            "ConceptoMovimiento": "RETIRO ATM SaaS",
+            "TipoMovimientoCargoAbono": "Cargo",
+            "ImporteMovimiento": "100.0000",
+            "MonedaMovimiento": "MXN",
+            "Referencia": "",
+            "Observaciones": ""
+        }</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Datos de la prueba</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>___________________________</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Colectiva: Prueba SAAS
+Tarjeta: 9900012000263004
+Monto: $100.00
+Saldo Actual SaaS: $1,047.50
+Saldo Actual TH: $1,814.80</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Datos de la prueba</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>___________________________</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Colectiva: Prueba SAAS
+Tarjeta: 9900012000263004
+Monto: $2,000.00
+Saldo Actual SaaS: $947.50
+Saldo Actual TH:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>$1,714.80</t>
     </r>
   </si>
 </sst>
@@ -1476,6 +1871,407 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>117431</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>130479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8319601</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>3226536</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BA2EF80-A4BD-1EA8-C120-A742CA5B85E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20080787" y="12617363"/>
+          <a:ext cx="8202170" cy="3096057"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>156575</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>195719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8244429</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2824986</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E66618FF-7DCA-3616-1435-4A6F16EA4F73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20119931" y="17562534"/>
+          <a:ext cx="8087854" cy="2629267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>130479</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>169623</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6093961</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>550676</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F51C1DA5-CF34-90D5-1198-7CDA0A705194}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15918493" y="17536438"/>
+          <a:ext cx="5963482" cy="381053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>143527</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>156576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8288539</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2833475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF2345B4-B3DE-46D2-58E9-5595B4E3CA75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22612089" y="22403323"/>
+          <a:ext cx="8145012" cy="2676899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247911</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>182671</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8440554</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>2888149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{268B19C8-2FCF-644C-FA03-04AB21BF06C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22716473" y="27309349"/>
+          <a:ext cx="8192643" cy="2705478"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>117432</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>117431</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6071388</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>517537</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0F6F4DB-A18C-65D9-DB6C-A78E451A8FF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15905446" y="27244109"/>
+          <a:ext cx="5953956" cy="400106"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>156574</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>130480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8349217</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>2845484</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F7E45A7-0138-274C-D2D0-B5576B3F8D1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22625136" y="2857501"/>
+          <a:ext cx="8192643" cy="2715004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>195719</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>143528</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8378836</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2829953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15DC1CC0-5A6E-7236-6906-47855155888E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22664281" y="7750480"/>
+          <a:ext cx="8183117" cy="2686425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>156576</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>143527</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6072427</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>524580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40260088-6824-7151-CEF3-169412837AAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15944590" y="7750479"/>
+          <a:ext cx="5915851" cy="381053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1987,10 +2783,10 @@
   <dimension ref="A1:J883"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="3" x14ac:dyDescent="0.2"/>
@@ -2003,7 +2799,7 @@
     <col min="6" max="6" width="14.85546875" style="39" customWidth="1"/>
     <col min="7" max="7" width="52.42578125" style="34" customWidth="1"/>
     <col min="8" max="8" width="62.7109375" style="37" customWidth="1"/>
-    <col min="9" max="9" width="62.7109375" style="34" customWidth="1"/>
+    <col min="9" max="9" width="100.28515625" style="34" customWidth="1"/>
     <col min="10" max="10" width="229.42578125" style="37" customWidth="1"/>
     <col min="11" max="16384" width="14.42578125" style="24"/>
   </cols>
@@ -2288,7 +3084,7 @@
         <v>58</v>
       </c>
       <c r="E14" s="54" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F14" s="55" t="s">
         <v>17</v>
@@ -2299,7 +3095,9 @@
       <c r="H14" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="70"/>
+      <c r="I14" s="70" t="s">
+        <v>87</v>
+      </c>
       <c r="J14" s="71"/>
     </row>
     <row r="15" spans="1:10" ht="384.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -2312,7 +3110,7 @@
         <v>59</v>
       </c>
       <c r="E15" s="54" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="F15" s="66" t="s">
         <v>17</v>
@@ -2336,7 +3134,7 @@
         <v>64</v>
       </c>
       <c r="E16" s="54" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="F16" s="55" t="s">
         <v>17</v>
@@ -2347,7 +3145,9 @@
       <c r="H16" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="70"/>
+      <c r="I16" s="70" t="s">
+        <v>81</v>
+      </c>
       <c r="J16" s="71"/>
     </row>
     <row r="17" spans="1:10" ht="384.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -2360,7 +3160,7 @@
         <v>65</v>
       </c>
       <c r="E17" s="54" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="F17" s="66" t="s">
         <v>17</v>
@@ -2384,7 +3184,7 @@
         <v>66</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="F18" s="55" t="s">
         <v>17</v>
@@ -2395,7 +3195,9 @@
       <c r="H18" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I18" s="70"/>
+      <c r="I18" s="70" t="s">
+        <v>82</v>
+      </c>
       <c r="J18" s="71"/>
     </row>
     <row r="19" spans="1:10" ht="384.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -2408,7 +3210,7 @@
         <v>67</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F19" s="66" t="s">
         <v>17</v>
@@ -12765,7 +13567,8 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
file: Se agrega documentacion de los casos de uso faltantes
</commit_message>
<xml_diff>
--- a/HU061 Matriz de Pruebas.xlsx
+++ b/HU061 Matriz de Pruebas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo\DNU\Documentacion\HU061 Cuenta Eje SAAS en Prepago SAAS ES\Repo\HU061_Desarrollo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragdn\OneDrive\Documentos\Cacao\Requerimientos\HU061 - Cuenta Eje SAAS ES\Desarrollo\HU061_Desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC20B656-8F2E-4444-B090-46AC3438FC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C059F896-8DC0-4E7C-9CDF-332FD36BFB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ciclo 1" sheetId="3" r:id="rId1"/>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="111">
   <si>
     <t>Totem</t>
   </si>
@@ -452,86 +452,6 @@
   </si>
   <si>
     <t>La transacción deberá ser rechazada, dado que el monto excede el saldo actual de la cuenta.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Datos de la prueba___________________________
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Colectiva:
-Tarjeta:
-Monto:
-Saldo:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Datos de la prueba</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>___________________________</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Colectiva:
-Tarjeta:
-Monto:
-Saldo:</t>
-    </r>
   </si>
   <si>
     <t>Permitir Transacción para un cuenta habiente de una empresa.</t>
@@ -1535,6 +1455,275 @@
 [2022-06-20 16:26:17.802] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] autorizaOperacion(): autorizador.Exceptions.AutorizadorGenericException: [ID_Mensaje:02101109103206400000112345678094201085000100201] Ocurrio un error al Ejecutar el Evento [SAAS01] No se generaron Polizas que reversar
 [2022-06-20 16:26:17.802] [ERROR] El Evento+MTI :isoPlugInEVERTEC12730210 , Responde con el Formato por Default</t>
   </si>
+  <si>
+    <t>2022-06-20 14:04:48.830] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Mensaje ISO8583 - NO SE DETIENE LA OPERACION PERO NO SE PUDO DECODIFICAR EL CAMPO 48
+[2022-06-20 14:04:48.830] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001]null
+[2022-06-20 14:04:48.830] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] El Mensaje ISO recibido no tiene el Campo [108] definido.
+[2022-06-20 14:04:48.830] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Ocurrio un Error al Obtenet los Tokens del Mensaje ISO8583 , Token :@TKNC6_1, SubElement : 1, LosValores :  MCC01105S MCC01105S
+[2022-06-20 14:04:48.830] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Ocurrio un Error al Obtenet los Tokens del Mensaje ISO8583 , Token :@TKNC6_2, SubElement : 2, LosValores :  MCC01105S MCC01105S
+[2022-06-20 14:04:48.846] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] insertaDetallesPoliza(): 1016-SALDO INSUFICIENTE EN CUENTA DE CLIENTE CUENTAHABIENTE; ID_Cuenta: 1015537, ID_Colectiva:212102, ID_TipoColectiva:10, ID_TipoCuenta:3, ID_CadenaComercial:212099
+[2022-06-20 14:04:48.846] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001]autorizador.Exceptions.SaldoInsuficienteException: LA CUENTA NO TIENE SALDO SUFICIENTE PARA GENERAR EL MOVIMIENTO SOLICITADO
+[2022-06-20 14:04:48.846] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Poliza no creada: RETIRO ATM SaaS Codigo de Respuesta: 51
+[2022-06-20 14:04:48.846] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] autorizaOperacion(): autorizador.Exceptions.AutorizadorGenericException: [ID_Mensaje:02101109103206400000112345678094003085000100001] Ocurrio un error al Ejecutar el Evento [SAAS03] No se generaron Polizas que reversar
+[</t>
+  </si>
+  <si>
+    <t>2022-06-20 13:50:28.595] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Mensaje ISO8583 - NO SE DETIENE LA OPERACION PERO NO SE PUDO DECODIFICAR EL CAMPO 48
+[2022-06-20 13:50:28.595] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001]null
+[2022-06-20 13:50:28.595] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] El Mensaje ISO recibido no tiene el Campo [108] definido.
+[2022-06-20 13:50:28.595] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Ocurrio un Error al Obtenet los Tokens del Mensaje ISO8583 , Token :@TKNC6_1, SubElement : 1, LosValores :  MCC01105S MCC01105S
+[2022-06-20 13:50:28.595] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Ocurrio un Error al Obtenet los Tokens del Mensaje ISO8583 , Token :@TKNC6_2, SubElement : 2, LosValores :  MCC01105S MCC01105S
+[2022-06-20 13:50:28.626] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] insertaDetallesPoliza(): 1016-SALDO INSUFICIENTE EN CUENTA DE CLIENTE CUENTAHABIENTE; ID_Cuenta: 1015543, ID_Colectiva:212103, ID_TipoColectiva:10, ID_TipoCuenta:3, ID_CadenaComercial:212098
+[2022-06-20 13:50:28.626] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001]autorizador.Exceptions.SaldoInsuficienteException: LA CUENTA NO TIENE SALDO SUFICIENTE PARA GENERAR EL MOVIMIENTO SOLICITADO
+[2022-06-20 13:50:28.626] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Poliza no creada: RETIRO ATM SaaS Codigo de Respuesta: 51
+[2022-06-20 13:50:28.626] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] autorizaOperacion(): autorizador.Exceptions.AutorizadorGenericException: [ID_Mensaje:02101109103206400000112345678094003085000100001] Ocurrio un error al Ejecutar el Evento [SAAS03] No se generaron Polizas que reversar
+[</t>
+  </si>
+  <si>
+    <t>[2022-06-20 14:16:00.188] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Mensaje ISO8583 - NO SE DETIENE LA OPERACION PERO NO SE PUDO DECODIFICAR EL CAMPO 48
+[2022-06-20 14:16:00.188] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001]null
+[2022-06-20 14:16:00.188] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] El Mensaje ISO recibido no tiene el Campo [108] definido.
+[2022-06-20 14:16:00.188] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Ocurrio un Error al Obtenet los Tokens del Mensaje ISO8583 , Token :@TKNC6_1, SubElement : 1, LosValores :  MCC01105S MCC01105S
+[2022-06-20 14:16:00.188] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Ocurrio un Error al Obtenet los Tokens del Mensaje ISO8583 , Token :@TKNC6_2, SubElement : 2, LosValores :  MCC01105S MCC01105S
+[2022-06-20 14:16:00.219] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] insertaDetallesPoliza(): 1016-SALDO INSUFICIENTE EN CUENTA DE CLIENTE CUENTAHABIENTE; ID_Cuenta: 668435, ID_Colectiva:148553, ID_TipoColectiva:10, ID_TipoCuenta:3, ID_CadenaComercial:148552
+[2022-06-20 14:16:00.219] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001]autorizador.Exceptions.SaldoInsuficienteException: LA CUENTA NO TIENE SALDO SUFICIENTE PARA GENERAR EL MOVIMIENTO SOLICITADO
+[2022-06-20 14:16:00.219] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] Poliza no creada: RETIRO ATM SaaS Codigo de Respuesta: 51
+[2022-06-20 14:16:00.219] [ERROR] [ID_Mensaje:02101109103206400000112345678094003085000100001] autorizaOperacion(): autorizador.Exceptions.AutorizadorGenericException: [ID_Mensaje:02101109103206400000112345678094003085000100001] Ocurrio un error al Ejecutar el Evento [SAAS03] No se generaron Polizas que reversar</t>
+  </si>
+  <si>
+    <t>{
+            "ImporteOrigenMovimiento": "15.0000",
+            "MonedaOrigenMovimiento": "484",
+            "NumeroAfiliacionComercio": "0000000",
+            "DescripcionComercio": "Member Financial Instis",
+            "PaisComercio": "484",
+            "DescripcionPais": "México",
+            "SaldoDespuesMovimiento": "480.50",
+            "ClaveMovimiento": "PB46",
+            "MCC": "6011",
+            "EstatusPostOperacion": "004",
+            "DescripcionPostOperacion": "EN TRANSITO",
+            "Autorizacion": "001899",
+            "IDMovimiento": "1393360",
+            "FechaMovimiento": "2022-06-20 16:53:27",
+            "ConceptoMovimiento": "COMPRA SaaS",
+            "TipoMovimientoCargoAbono": "Cargo",
+            "ImporteMovimiento": "15.0000",
+            "MonedaMovimiento": "MXN",
+            "Referencia": "",
+            "Observaciones": ""
+        }</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Datos de la prueba</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>___________________________</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Colectiva: Empresa Debito Prueba SAAS
+Tarjeta: 9900012011858860
+Monto: $15.00
+Saldo Actual SaaS: $702.47
+Saldo Actual TH: $495.00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Datos de la prueba___________________________
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Colectiva: Empresa Debito Prueba SAAS
+Tarjeta: 9900012011858860
+Monto: $500.00
+Saldo Actual SaaS: $687.47
+Saldo Actual TH: $480.50</t>
+    </r>
+  </si>
+  <si>
+    <t>[2022-06-20 16:57:27.435] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] El Mensaje ISO recibido no tiene el Campo [108] definido.
+[2022-06-20 16:57:27.450] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] Ocurrio un Error al Obtenet los Tokens del Mensaje ISO8583 , Token :@TKNC6_1, SubElement : 1, LosValores :  MCC01105S MCC01105S
+[2022-06-20 16:57:27.450] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] Ocurrio un Error al Obtenet los Tokens del Mensaje ISO8583 , Token :@TKNC6_2, SubElement : 2, LosValores :  MCC01105S MCC01105S
+[2022-06-20 16:57:27.450] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] ejecutaRegla(): Respuesta de la Regla [regla_ValidaMedioAcceso]: REGLA AUTORIZADA
+[2022-06-20 16:57:27.466] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] insertaDetallesPoliza(): 1016-SALDO INSUFICIENTE EN CUENTA DE CLIENTE CUENTAHABIENTE; ID_Cuenta: 1015543, ID_Colectiva:212103, ID_TipoColectiva:10, ID_TipoCuenta:3, ID_CadenaComercial:212098
+[2022-06-20 16:57:27.466] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201]autorizador.Exceptions.SaldoInsuficienteException: LA CUENTA NO TIENE SALDO SUFICIENTE PARA GENERAR EL MOVIMIENTO SOLICITADO
+[2022-06-20 16:57:27.466] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] Poliza no creada: COMPRA SaaS Codigo de Respuesta: 51
+[2022-06-20 16:57:27.466] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] autorizaOperacion(): autorizador.Exceptions.AutorizadorGenericException: [ID_Mensaje:02101109103206400000112345678094201085000100201] Ocurrio un error al Ejecutar el Evento [SAAS01] No se generaron Polizas que reversar</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Datos de la prueba</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>___________________________</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Colectiva: Subempresa Debito Prueba SAAS
+Tarjeta: 9900012046474446
+Monto: $50.00
+Saldo Actual SaaS: $687.47
+Saldo Actual TH: $495.00</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+            "ImporteOrigenMovimiento": "50.0000",
+            "MonedaOrigenMovimiento": "484",
+            "NumeroAfiliacionComercio": "0000000",
+            "DescripcionComercio": "Member Financial Instis",
+            "PaisComercio": "484",
+            "DescripcionPais": "México",
+            "SaldoDespuesMovimiento": "445.00",
+            "ClaveMovimiento": "PB46",
+            "MCC": "6011",
+            "EstatusPostOperacion": "004",
+            "DescripcionPostOperacion": "EN TRANSITO",
+            "Autorizacion": "001900",
+            "IDMovimiento": "1393362",
+            "FechaMovimiento": "2022-06-20 17:01:09",
+            "ConceptoMovimiento": "COMPRA SaaS",
+            "TipoMovimientoCargoAbono": "Cargo",
+            "ImporteMovimiento": "50.0000",
+            "MonedaMovimiento": "MXN",
+            "Referencia": "",
+            "Observaciones": ""
+        }</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.- Contar con acceso y permisos necesarios para Central Administrativa 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Datos de la prueba___________________________
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Colectiva: Subempresa Debito Prueba SAAS
+Tarjeta: 9900012046474446
+Monto: $500.00
+Saldo Actual SaaS: $637.47
+Saldo Actual TH: $445.00</t>
+    </r>
+  </si>
+  <si>
+    <t>[2022-06-20 17:05:46.135] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] Mensaje ISO8583 - NO SE DETIENE LA OPERACION PERO NO SE PUDO DECODIFICAR EL CAMPO 48
+[2022-06-20 17:05:46.135] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201]null
+[2022-06-20 17:05:46.135] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] El Mensaje ISO recibido no tiene el Campo [108] definido.
+[2022-06-20 17:05:46.135] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] Ocurrio un Error al Obtenet los Tokens del Mensaje ISO8583 , Token :@TKNC6_1, SubElement : 1, LosValores :  MCC01105S MCC01105S
+[2022-06-20 17:05:46.135] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] Ocurrio un Error al Obtenet los Tokens del Mensaje ISO8583 , Token :@TKNC6_2, SubElement : 2, LosValores :  MCC01105S MCC01105S
+[2022-06-20 17:05:46.135] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] ejecutaRegla(): Respuesta de la Regla [regla_ValidaMedioAcceso]: REGLA AUTORIZADA
+[2022-06-20 17:05:46.167] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] insertaDetallesPoliza(): 1016-SALDO INSUFICIENTE EN CUENTA DE CLIENTE CUENTAHABIENTE; ID_Cuenta: 1015537, ID_Colectiva:212102, ID_TipoColectiva:10, ID_TipoCuenta:3, ID_CadenaComercial:212099
+[2022-06-20 17:05:46.167] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201]autorizador.Exceptions.SaldoInsuficienteException: LA CUENTA NO TIENE SALDO SUFICIENTE PARA GENERAR EL MOVIMIENTO SOLICITADO
+[2022-06-20 17:05:46.167] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] Poliza no creada: COMPRA SaaS Codigo de Respuesta: 51
+[2022-06-20 17:05:46.182] [ERROR] [ID_Mensaje:02101109103206400000112345678094201085000100201] autorizaOperacion(): autorizador.Exceptions.AutorizadorGenericException: [ID_Mensaje:02101109103206400000112345678094201085000100201] Ocurrio un error al Ejecutar el Evento [SAAS01] No se generaron Polizas que reversar</t>
+  </si>
 </sst>
 </file>
 
@@ -2415,50 +2604,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>130479</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>169623</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>6093961</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>550676</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F51C1DA5-CF34-90D5-1198-7CDA0A705194}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15918493" y="17536438"/>
-          <a:ext cx="5963482" cy="381053"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>143527</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -2484,7 +2629,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2528,7 +2673,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2537,50 +2682,6 @@
         <a:xfrm>
           <a:off x="22716473" y="27309349"/>
           <a:ext cx="8192643" cy="2705478"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>117432</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>117431</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>6071388</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>517537</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagen 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0F6F4DB-A18C-65D9-DB6C-A78E451A8FF4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15905446" y="27244109"/>
-          <a:ext cx="5953956" cy="400106"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2616,7 +2717,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2660,7 +2761,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2669,50 +2770,6 @@
         <a:xfrm>
           <a:off x="22664281" y="7750480"/>
           <a:ext cx="8183117" cy="2686425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>156576</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>143527</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>6072427</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>524580</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Imagen 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40260088-6824-7151-CEF3-169412837AAE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15944590" y="7750479"/>
-          <a:ext cx="5915851" cy="381053"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2748,7 +2805,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2792,7 +2849,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2836,7 +2893,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2880,7 +2937,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2924,7 +2981,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2968,7 +3025,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3012,7 +3069,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3056,7 +3113,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3100,7 +3157,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3109,6 +3166,182 @@
         <a:xfrm>
           <a:off x="22468562" y="37173596"/>
           <a:ext cx="8219048" cy="4200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>195719</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>156575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8407415</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>2871579</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Imagen 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA977441-075B-EC4C-81B9-7270C660D908}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22664281" y="71489691"/>
+          <a:ext cx="8211696" cy="2715004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>221815</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>208767</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8414458</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>2904718</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Imagen 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEAD943B-A456-DE98-9B00-DDDA50D67AC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22690377" y="76421815"/>
+          <a:ext cx="8192643" cy="2695951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>182671</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>143528</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8461051</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>2887111</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Imagen 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{527F1080-E3B7-DCF0-6BAB-2A57CF93CFC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22651233" y="81236507"/>
+          <a:ext cx="8278380" cy="2743583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>208767</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>195719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8410937</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>2910723</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Imagen 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44A2F428-E655-2A70-AEEE-16146A7C4090}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22677329" y="86168630"/>
+          <a:ext cx="8202170" cy="2715004"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3633,10 +3866,10 @@
   <dimension ref="A1:J883"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="3" x14ac:dyDescent="0.2"/>
@@ -3778,19 +4011,19 @@
         <v>58</v>
       </c>
       <c r="E7" s="54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F7" s="55" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="54" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H7" s="54" t="s">
         <v>60</v>
       </c>
       <c r="I7" s="54" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J7" s="54"/>
     </row>
@@ -3804,19 +4037,19 @@
         <v>59</v>
       </c>
       <c r="E8" s="54" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F8" s="66" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="65" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H8" s="67" t="s">
         <v>61</v>
       </c>
       <c r="I8" s="65" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J8" s="67"/>
     </row>
@@ -3827,22 +4060,22 @@
       <c r="B9" s="65"/>
       <c r="C9" s="65"/>
       <c r="D9" s="54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E9" s="54" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F9" s="55" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H9" s="54" t="s">
         <v>60</v>
       </c>
       <c r="I9" s="65" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J9" s="67"/>
     </row>
@@ -3853,22 +4086,22 @@
       <c r="B10" s="65"/>
       <c r="C10" s="65"/>
       <c r="D10" s="65" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F10" s="66" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H10" s="67" t="s">
         <v>61</v>
       </c>
       <c r="I10" s="65" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J10" s="67"/>
     </row>
@@ -3879,22 +4112,22 @@
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
       <c r="D11" s="54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F11" s="55" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H11" s="54" t="s">
         <v>60</v>
       </c>
       <c r="I11" s="65" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J11" s="67"/>
     </row>
@@ -3905,22 +4138,22 @@
       <c r="B12" s="65"/>
       <c r="C12" s="65"/>
       <c r="D12" s="65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E12" s="54" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F12" s="66" t="s">
         <v>17</v>
       </c>
       <c r="G12" s="65" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H12" s="67" t="s">
         <v>61</v>
       </c>
       <c r="I12" s="65" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J12" s="67"/>
     </row>
@@ -3950,19 +4183,19 @@
         <v>58</v>
       </c>
       <c r="E14" s="54" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F14" s="55" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H14" s="54" t="s">
         <v>60</v>
       </c>
       <c r="I14" s="70" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J14" s="71"/>
     </row>
@@ -3976,18 +4209,20 @@
         <v>59</v>
       </c>
       <c r="E15" s="54" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F15" s="66" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="65" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H15" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="70"/>
+      <c r="I15" s="70" t="s">
+        <v>102</v>
+      </c>
       <c r="J15" s="71"/>
     </row>
     <row r="16" spans="1:10" ht="384.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -3997,22 +4232,22 @@
       <c r="B16" s="58"/>
       <c r="C16" s="57"/>
       <c r="D16" s="54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E16" s="54" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F16" s="55" t="s">
         <v>17</v>
       </c>
       <c r="G16" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H16" s="54" t="s">
         <v>60</v>
       </c>
       <c r="I16" s="70" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J16" s="71"/>
     </row>
@@ -4023,21 +4258,23 @@
       <c r="B17" s="58"/>
       <c r="C17" s="57"/>
       <c r="D17" s="65" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E17" s="54" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F17" s="66" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="65" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H17" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="70"/>
+      <c r="I17" s="70" t="s">
+        <v>101</v>
+      </c>
       <c r="J17" s="71"/>
     </row>
     <row r="18" spans="1:10" ht="384.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4047,22 +4284,22 @@
       <c r="B18" s="58"/>
       <c r="C18" s="57"/>
       <c r="D18" s="54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F18" s="55" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H18" s="54" t="s">
         <v>60</v>
       </c>
       <c r="I18" s="70" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J18" s="71"/>
     </row>
@@ -4073,21 +4310,23 @@
       <c r="B19" s="58"/>
       <c r="C19" s="57"/>
       <c r="D19" s="65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F19" s="66" t="s">
         <v>17</v>
       </c>
       <c r="G19" s="65" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H19" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="I19" s="70"/>
+      <c r="I19" s="70" t="s">
+        <v>100</v>
+      </c>
       <c r="J19" s="71"/>
     </row>
     <row r="20" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4116,19 +4355,19 @@
         <v>58</v>
       </c>
       <c r="E21" s="54" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F21" s="55" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="54" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H21" s="54" t="s">
         <v>60</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J21" s="30"/>
     </row>
@@ -4142,19 +4381,19 @@
         <v>59</v>
       </c>
       <c r="E22" s="54" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F22" s="66" t="s">
         <v>17</v>
       </c>
       <c r="G22" s="65" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H22" s="67" t="s">
         <v>61</v>
       </c>
       <c r="I22" s="28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J22" s="30"/>
     </row>
@@ -4165,21 +4404,23 @@
       <c r="B23" s="29"/>
       <c r="C23" s="26"/>
       <c r="D23" s="54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E23" s="54" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="F23" s="55" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="54" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H23" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I23" s="28"/>
+      <c r="I23" s="28" t="s">
+        <v>103</v>
+      </c>
       <c r="J23" s="30"/>
     </row>
     <row r="24" spans="1:10" ht="384.75" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -4189,21 +4430,23 @@
       <c r="B24" s="29"/>
       <c r="C24" s="26"/>
       <c r="D24" s="65" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" s="54" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="F24" s="66" t="s">
         <v>17</v>
       </c>
       <c r="G24" s="65" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H24" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="I24" s="28"/>
+      <c r="I24" s="28" t="s">
+        <v>106</v>
+      </c>
       <c r="J24" s="30"/>
     </row>
     <row r="25" spans="1:10" ht="384.75" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -4213,21 +4456,23 @@
       <c r="B25" s="29"/>
       <c r="C25" s="26"/>
       <c r="D25" s="54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E25" s="54" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="F25" s="55" t="s">
         <v>17</v>
       </c>
       <c r="G25" s="54" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H25" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I25" s="28"/>
+      <c r="I25" s="28" t="s">
+        <v>108</v>
+      </c>
       <c r="J25" s="30"/>
     </row>
     <row r="26" spans="1:10" ht="384.75" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -4237,21 +4482,23 @@
       <c r="B26" s="29"/>
       <c r="C26" s="26"/>
       <c r="D26" s="65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E26" s="54" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="F26" s="66" t="s">
         <v>17</v>
       </c>
       <c r="G26" s="65" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H26" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="I26" s="28"/>
+      <c r="I26" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="J26" s="30"/>
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>